<commit_message>
Updated RCI wine calculator
</commit_message>
<xml_diff>
--- a/files/assets/files/RCI-Wine-Package-Analysis.xlsx
+++ b/files/assets/files/RCI-Wine-Package-Analysis.xlsx
@@ -14,11 +14,12 @@
     <definedName name="All_Types">'Wine Packages'!$A$15:$A$19</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>Wine Packages</t>
   </si>
@@ -310,6 +311,12 @@
   </si>
   <si>
     <t>ie, how much do I save, compared to buying the bottles outside the package?)</t>
+  </si>
+  <si>
+    <t>Gratuity?</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -508,29 +515,29 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -545,9 +552,6 @@
     <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -564,15 +568,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -593,6 +588,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -628,27 +629,33 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E7" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E7" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A3:E7">
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Bottles" dataDxfId="0"/>
-    <tableColumn id="2" name="USD inc. Gratuity" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="1" name="Bottles" dataDxfId="7"/>
+    <tableColumn id="2" name="USD inc. Gratuity" dataDxfId="6" dataCellStyle="Currency"/>
     <tableColumn id="3" name="Package Cost per Bottle" dataDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>B4/A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Average Saving *" dataDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="4" name="Average Saving *" dataDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])-Table2[[#This Row],[USD inc. Gratuity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="% Saving **" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="5" name="% Saving **" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -657,7 +664,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Variety"/>
@@ -665,8 +672,8 @@
     <tableColumn id="3" name="Region"/>
     <tableColumn id="4" name="Country"/>
     <tableColumn id="5" name="Class"/>
-    <tableColumn id="6" name="No Grat." dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="7" name="Inc Grat." dataDxfId="7" dataCellStyle="Currency">
+    <tableColumn id="6" name="No Grat." dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="7" name="Inc Grat." dataDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*(1+'Wine Packages'!$B$9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -962,7 +969,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -978,21 +985,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="G1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:8" ht="19.5" thickTop="1">
+      <c r="G2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="3" spans="1:8" ht="30">
       <c r="A3" s="2" t="s">
         <v>2</v>
@@ -1095,48 +1109,48 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="12">
         <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="17" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="42" customHeight="1" thickBot="1">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1145,7 +1159,7 @@
         <v>83</v>
       </c>
       <c r="B15" s="3">
-        <f>AVERAGE(Table1[Inc Grat.])</f>
+        <f>IF($H$2="Yes",AVERAGE(Table1[Inc Grat.]),AVERAGE(Table1[No Grat.]))</f>
         <v>52.078571428571422</v>
       </c>
     </row>
@@ -1154,7 +1168,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="3">
-        <f>AVERAGEIF(Table1[Class],"=Sparkling",Table1[Inc Grat.])</f>
+        <f>IF($H$2="Yes",AVERAGEIF(Table1[Class],"=Sparkling",Table1[Inc Grat.]),AVERAGEIF(Table1[Class],"=Sparkling",Table1[No Grat.]))</f>
         <v>51.174999999999997</v>
       </c>
     </row>
@@ -1163,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <f>AVERAGEIF(Table1[Class],"=White",Table1[Inc Grat.])</f>
+        <f>IF($H$2="Yes",AVERAGEIF(Table1[Class],"=White",Table1[Inc Grat.]),AVERAGEIF(Table1[Class],"=White",Table1[No Grat.]))</f>
         <v>49.705555555555549</v>
       </c>
     </row>
@@ -1172,7 +1186,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="3">
-        <f>AVERAGEIF(Table1[Class],"=Red",Table1[Inc Grat.])</f>
+        <f>IF($H$2="Yes",AVERAGEIF(Table1[Class],"=Red",Table1[Inc Grat.]),AVERAGEIF(Table1[Class],"=Red",Table1[No Grat.]))</f>
         <v>54.394999999999996</v>
       </c>
     </row>
@@ -1181,34 +1195,37 @@
         <v>78</v>
       </c>
       <c r="B19" s="3">
-        <f>AVERAGEIF(Table1[Class],"&lt;&gt;Sparkling",Table1[Inc Grat.])</f>
+        <f>IF($H$2="Yes",AVERAGEIF(Table1[Class],"&lt;&gt;Sparkling",Table1[Inc Grat.]),AVERAGEIF(Table1[Class],"&lt;&gt;Sparkling",Table1[No Grat.]))</f>
         <v>52.173684210526318</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="F10:G11"/>
     <mergeCell ref="A23:G23"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
       <formula1>All_Types</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1326,10 +1343,10 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>43</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <f>F4*(1+'Wine Packages'!$B$9)</f>
         <v>49.449999999999996</v>
       </c>
@@ -1350,10 +1367,10 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>43</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <f>F5*(1+'Wine Packages'!$B$9)</f>
         <v>49.449999999999996</v>
       </c>
@@ -1614,10 +1631,10 @@
       <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>48</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <f>F16*(1+'Wine Packages'!$B$9)</f>
         <v>55.199999999999996</v>
       </c>
@@ -1767,16 +1784,16 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="F27" s="10"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="F28" s="10"/>
+      <c r="F28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to change text to indicate gratuity included or not
</commit_message>
<xml_diff>
--- a/files/assets/files/RCI-Wine-Package-Analysis.xlsx
+++ b/files/assets/files/RCI-Wine-Package-Analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>Wine Packages</t>
   </si>
@@ -265,34 +265,6 @@
   </si>
   <si>
     <t>Average Saving *</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Average costs per bottle </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(inc. Gratuity)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
   </si>
   <si>
     <t>All Types</t>
@@ -522,6 +494,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -535,9 +510,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -969,7 +941,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -985,15 +957,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="G1" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>78</v>
@@ -1001,10 +973,10 @@
     </row>
     <row r="2" spans="1:8" ht="19.5" thickTop="1">
       <c r="G2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
@@ -1117,46 +1089,47 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A11" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A11" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="42" customHeight="1" thickBot="1">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A13" s="9" t="s">
-        <v>82</v>
+      <c r="A13" s="9" t="str">
+        <f>CONCATENATE("Average costs per bottle (", IF($H$2="Yes","inc. Gratuity","NO Gratuity"), ")")</f>
+        <v>Average costs per bottle (inc. Gratuity)</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3">
         <f>IF($H$2="Yes",AVERAGE(Table1[Inc Grat.]),AVERAGE(Table1[No Grat.]))</f>
@@ -1200,15 +1173,15 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="A23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Changed column titles to be more accurate
</commit_message>
<xml_diff>
--- a/files/assets/files/RCI-Wine-Package-Analysis.xlsx
+++ b/files/assets/files/RCI-Wine-Package-Analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="35540" windowHeight="21020"/>
   </bookViews>
   <sheets>
     <sheet name="Wine Packages" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,13 @@
   <definedNames>
     <definedName name="All_Types">'Wine Packages'!$A$15:$A$19</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -261,12 +266,6 @@
     <t>Package Cost per Bottle</t>
   </si>
   <si>
-    <t>% Saving **</t>
-  </si>
-  <si>
-    <t>Average Saving *</t>
-  </si>
-  <si>
     <t>All Types</t>
   </si>
   <si>
@@ -289,16 +288,22 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Average % Saving **</t>
+  </si>
+  <si>
+    <t>Average USD$ Saving *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,7 +564,7 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -602,10 +607,10 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,20 +619,17 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E7" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A3:E7">
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
+  <autoFilter ref="A3:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Bottles" dataDxfId="7"/>
     <tableColumn id="2" name="USD inc. Gratuity" dataDxfId="6" dataCellStyle="Currency"/>
     <tableColumn id="3" name="Package Cost per Bottle" dataDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>B4/A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Average Saving *" dataDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="4" name="Average USD$ Saving *" dataDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])-Table2[[#This Row],[USD inc. Gratuity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="% Saving **" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="5" name="Average % Saving **" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -937,26 +939,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1">
+    <row r="1" spans="1:8" ht="20" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -965,21 +967,21 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="G1" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickTop="1">
+    <row r="2" spans="1:8" ht="19" thickTop="1">
       <c r="G2" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -990,10 +992,10 @@
         <v>79</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1090,20 +1092,20 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="31.5" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -1121,7 +1123,7 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickTop="1">
+    <row r="13" spans="1:8" ht="15" thickTop="1">
       <c r="A13" s="9" t="str">
         <f>CONCATENATE("Average costs per bottle (", IF($H$2="Yes","inc. Gratuity","NO Gratuity"), ")")</f>
         <v>Average costs per bottle (inc. Gratuity)</v>
@@ -1129,7 +1131,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3">
         <f>IF($H$2="Yes",AVERAGE(Table1[Inc Grat.]),AVERAGE(Table1[No Grat.]))</f>
@@ -1174,7 +1176,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1193,7 +1195,7 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1">
       <formula1>All_Types</formula1>
     </dataValidation>
@@ -1205,28 +1207,33 @@
     <hyperlink ref="A23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1">
@@ -1773,5 +1780,10 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed pendantic mis-calculation on percentage column
</commit_message>
<xml_diff>
--- a/files/assets/files/RCI-Wine-Package-Analysis.xlsx
+++ b/files/assets/files/RCI-Wine-Package-Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="35540" windowHeight="21020"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="35540" windowHeight="21020"/>
   </bookViews>
   <sheets>
     <sheet name="Wine Packages" sheetId="1" r:id="rId1"/>
@@ -530,6 +530,9 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -565,9 +568,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -629,8 +629,8 @@
     <tableColumn id="4" name="Average USD$ Saving *" dataDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])-Table2[[#This Row],[USD inc. Gratuity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Average % Saving **" dataDxfId="3" dataCellStyle="Percent">
-      <calculatedColumnFormula>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</calculatedColumnFormula>
+    <tableColumn id="5" name="Average % Saving **" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table2[[#This Row],[Average USD$ Saving *]]/Table2[[#This Row],[USD inc. Gratuity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Variety"/>
@@ -646,8 +646,8 @@
     <tableColumn id="3" name="Region"/>
     <tableColumn id="4" name="Country"/>
     <tableColumn id="5" name="Class"/>
-    <tableColumn id="6" name="No Grat." dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="7" name="Inc Grat." dataDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="6" name="No Grat." dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" name="Inc Grat." dataDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*(1+'Wine Packages'!$B$9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -943,7 +943,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1015,9 +1015,10 @@
         <v>71.118421052631589</v>
       </c>
       <c r="E4" s="1">
-        <f>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</f>
-        <v>0.72737819025522032</v>
-      </c>
+        <f>Table2[[#This Row],[Average USD$ Saving *]]/Table2[[#This Row],[USD inc. Gratuity]]</f>
+        <v>0.3748006379585328</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4">
@@ -1036,8 +1037,8 @@
         <v>112.21578947368428</v>
       </c>
       <c r="E5" s="1">
-        <f>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</f>
-        <v>0.69274113357640021</v>
+        <f>Table2[[#This Row],[Average USD$ Saving *]]/Table2[[#This Row],[USD inc. Gratuity]]</f>
+        <v>0.44354066985645968</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1057,8 +1058,8 @@
         <v>176.73684210526312</v>
       </c>
       <c r="E6" s="1">
-        <f>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</f>
-        <v>0.66125290023201866</v>
+        <f>Table2[[#This Row],[Average USD$ Saving *]]/Table2[[#This Row],[USD inc. Gratuity]]</f>
+        <v>0.51228070175438589</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1078,8 +1079,8 @@
         <v>240.83421052631587</v>
       </c>
       <c r="E7" s="1">
-        <f>Table2[[#This Row],[USD inc. Gratuity]]/(VLOOKUP($H$1,$A$15:$B$19,2,FALSE)*Table2[[#This Row],[Bottles]])</f>
-        <v>0.6153325599381283</v>
+        <f>Table2[[#This Row],[Average USD$ Saving *]]/Table2[[#This Row],[USD inc. Gratuity]]</f>
+        <v>0.62513747054202706</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>